<commit_message>
SImplificación de codigo para carga al CMS
</commit_message>
<xml_diff>
--- a/ponderacion_factores.xlsx
+++ b/ponderacion_factores.xlsx
@@ -13,6 +13,7 @@
   <definedNames>
     <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Hoja1!$A$1:$X$1401</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Hoja1!$A$1:$X$1401</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">Hoja1!$A$1:$X$1401</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10815" uniqueCount="2410">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10816" uniqueCount="2410">
   <si>
     <t xml:space="preserve">DIMENSIÓN</t>
   </si>
@@ -7517,33 +7518,33 @@
   <dimension ref="A1:X1401"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A593" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A1217" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="G616" activeCellId="0" sqref="G616"/>
+      <selection pane="bottomLeft" activeCell="C1244" activeCellId="0" sqref="C1244"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="36.2064777327935"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="36.5263157894737"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="3.96356275303644"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.5668016194332"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="40.17004048583"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.6761133603239"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="40.5991902834008"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="3.96356275303644"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.5668016194332"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="51.417004048583"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.6761133603239"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="51.8461538461539"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="3.96356275303644"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="17.5668016194332"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="4.60728744939271"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="14.7813765182186"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="80.9838056680162"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="17.4615384615385"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="17.5668016194332"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="17.6761133603239"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="4.49797570850202"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="14.8906882591093"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="81.7327935222672"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="17.5668016194332"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="17.6761133603239"/>
     <col collapsed="false" hidden="false" max="15" min="15" style="0" width="6.31983805668016"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="21.2105263157895"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="21.3157894736842"/>
     <col collapsed="false" hidden="false" max="17" min="17" style="0" width="9.4251012145749"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="20.246963562753"/>
-    <col collapsed="false" hidden="false" max="24" min="19" style="0" width="12.5344129554656"/>
-    <col collapsed="false" hidden="false" max="1025" min="25" style="0" width="14.5668016194332"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="20.3522267206478"/>
+    <col collapsed="false" hidden="false" max="24" min="19" style="0" width="12.6396761133603"/>
+    <col collapsed="false" hidden="false" max="1025" min="25" style="0" width="14.6761133603239"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -71007,12 +71008,16 @@
       <c r="W1243" s="8"/>
       <c r="X1243" s="8"/>
     </row>
-    <row r="1244" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1244" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1244" s="8" t="s">
         <v>2062</v>
       </c>
-      <c r="B1244" s="8"/>
-      <c r="C1244" s="8"/>
+      <c r="B1244" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1244" s="8" t="n">
+        <v>3</v>
+      </c>
       <c r="D1244" s="8" t="s">
         <v>2118</v>
       </c>

</xml_diff>